<commit_message>
valid data in data xcl
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\OpenKart\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFF4928-F96A-4149-938C-A90FDE8E8F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C165A4B-0D21-421E-B14D-0DB5FDA2E097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9336" yWindow="1296" windowWidth="7764" windowHeight="8880" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>abc123@gmail.com</t>
-  </si>
-  <si>
-    <t>Valid</t>
   </si>
   <si>
     <t>Invalid</t>
@@ -482,7 +479,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -544,7 +541,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -555,7 +552,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>